<commit_message>
exit early on rendering if data is missing
</commit_message>
<xml_diff>
--- a/dist/assets/data/gaming.xlsx
+++ b/dist/assets/data/gaming.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/devlan/Repos/research/data-forensics/dist/assets/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B98F304A-CD84-2141-AFAB-05483F2043EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C49DA5D1-715B-EC44-9DA9-203F72C905EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="500" windowWidth="30380" windowHeight="14440"/>
+    <workbookView xWindow="120" yWindow="500" windowWidth="30380" windowHeight="14440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,12 +32,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Nick</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -50,7 +50,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0">
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -63,7 +63,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0">
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -76,7 +76,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0">
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -89,7 +89,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0">
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -102,7 +102,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0">
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -115,7 +115,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0" shapeId="0">
+    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -128,7 +128,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0" shapeId="0">
+    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -141,7 +141,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="0" shapeId="0">
+    <comment ref="S1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -154,7 +154,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="0" shapeId="0">
+    <comment ref="T1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -306,10 +306,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="172" formatCode="0.000"/>
-    <numFmt numFmtId="173" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -367,11 +367,11 @@
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="172" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="173" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="172" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="173" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -685,11 +685,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T71"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:T69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="F81" sqref="F81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -5598,36 +5598,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="N71" s="1">
-        <f>SUM(N2:N69)</f>
-        <v>39</v>
-      </c>
-      <c r="O71" s="1">
-        <f t="shared" ref="O71:T71" si="15">SUM(O2:O69)</f>
-        <v>5</v>
-      </c>
-      <c r="P71" s="1">
-        <f t="shared" si="15"/>
-        <v>49</v>
-      </c>
-      <c r="Q71" s="1">
-        <f t="shared" si="15"/>
-        <v>38</v>
-      </c>
-      <c r="R71" s="1">
-        <f t="shared" si="15"/>
-        <v>29</v>
-      </c>
-      <c r="S71" s="1">
-        <f t="shared" si="15"/>
-        <v>27</v>
-      </c>
-      <c r="T71" s="1">
-        <f t="shared" si="15"/>
-        <v>27</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5638,7 +5608,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -5655,7 +5625,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>